<commit_message>
Yield daily rate computation ok. all tsts ok
</commit_message>
<xml_diff>
--- a/test/testdata/testSBEarningUsdc.xlsx
+++ b/test/testdata/testSBEarningUsdc.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="106">
   <si>
     <t>User ID</t>
   </si>
@@ -258,17 +258,108 @@
   </si>
   <si>
     <t>2020-12-24 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-24 21:34:05</t>
+  </si>
+  <si>
+    <t>2020-12-24 20:34:05</t>
+  </si>
+  <si>
+    <t>2020-12-24 21:41:40</t>
+  </si>
+  <si>
+    <t>2020-12-24 20:41:40</t>
+  </si>
+  <si>
+    <t>Exchanged to 284.559 CHSB. The fees for the exchange was taken in the bought currency</t>
+  </si>
+  <si>
+    <t>Exchanged from 0.1387311 ETH</t>
+  </si>
+  <si>
+    <t>2020-12-24 21:54:12</t>
+  </si>
+  <si>
+    <t>2020-12-24 20:54:12</t>
+  </si>
+  <si>
+    <t>2020-12-24 21:56:30</t>
+  </si>
+  <si>
+    <t>2020-12-24 20:56:30</t>
+  </si>
+  <si>
+    <t>Exchanged to 12344.548 CHSB. The fees for the exchange was taken in the bought currency</t>
+  </si>
+  <si>
+    <t>Exchanged from 6.002 ETH</t>
+  </si>
+  <si>
+    <t>2020-12-25 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-25 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-26 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-26 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-26 20:17:56</t>
+  </si>
+  <si>
+    <t>2020-12-26 19:17:56</t>
+  </si>
+  <si>
+    <t>2020-12-26 20:23:11</t>
+  </si>
+  <si>
+    <t>2020-12-26 19:23:11</t>
+  </si>
+  <si>
+    <t>Exchanged to 491.692 CHSB. The fees for the exchange was taken in the bought currency</t>
+  </si>
+  <si>
+    <t>Exchanged from 0.2465338 ETH</t>
+  </si>
+  <si>
+    <t>2020-12-27 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-27 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-28 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-28 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-29 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-29 08:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-30 09:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-30 08:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#0.##"/>
     <numFmt numFmtId="165" formatCode="#0.#######"/>
     <numFmt numFmtId="166" formatCode="#0.###"/>
     <numFmt numFmtId="167" formatCode="#0.########"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -381,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -410,8 +501,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,14 +851,16 @@
   </sheetPr>
   <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="29.07421875" customWidth="1"/>
-    <col min="3" max="10" width="14.921875" customWidth="1"/>
+    <col min="3" max="8" width="14.921875" customWidth="1"/>
+    <col min="9" max="9" width="14.921875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.921875" customWidth="1"/>
     <col min="11" max="11" width="69.921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -784,19 +905,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="9" spans="1:11" ht="26.15" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
@@ -823,7 +944,7 @@
       <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -858,7 +979,7 @@
       <c r="H10" s="5">
         <v>0</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="16">
         <v>0.68641045000000001</v>
       </c>
       <c r="J10" s="5">
@@ -893,7 +1014,7 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="17">
         <v>16122.8887</v>
       </c>
       <c r="J11" s="5">
@@ -928,7 +1049,7 @@
       <c r="H12" s="5">
         <v>0</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="18">
         <v>0.41420797999999998</v>
       </c>
       <c r="J12" s="5">
@@ -963,7 +1084,7 @@
       <c r="H13" s="5">
         <v>0</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="16">
         <v>9.3869679999999997E-2</v>
       </c>
       <c r="J13" s="5">
@@ -998,7 +1119,7 @@
       <c r="H14" s="5">
         <v>0</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="16">
         <v>9.3869679999999997E-2</v>
       </c>
       <c r="J14" s="5">
@@ -1033,7 +1154,7 @@
       <c r="H15" s="5">
         <v>0</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="17">
         <v>2233.3677117978</v>
       </c>
       <c r="J15" s="5">
@@ -1068,7 +1189,7 @@
       <c r="H16" s="5">
         <v>0</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="18">
         <v>0.10212599999999999</v>
       </c>
       <c r="J16" s="5">
@@ -1103,7 +1224,7 @@
       <c r="H17" s="5">
         <v>0</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="16">
         <v>5.0977170000000002E-2</v>
       </c>
       <c r="J17" s="5">
@@ -1138,7 +1259,7 @@
       <c r="H18" s="5">
         <v>0</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="16">
         <v>5.0977170000000002E-2</v>
       </c>
       <c r="J18" s="5">
@@ -1173,7 +1294,7 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="17">
         <v>1215.440864899216</v>
       </c>
       <c r="J19" s="5">
@@ -1208,8 +1329,8 @@
       <c r="H20" s="5">
         <v>0</v>
       </c>
-      <c r="I20" s="5">
-        <v>9.3793520000000008</v>
+      <c r="I20" s="17">
+        <v>0.8</v>
       </c>
       <c r="J20" s="5">
         <v>9.3855199556687197</v>
@@ -1243,8 +1364,8 @@
       <c r="H21" s="5">
         <v>0</v>
       </c>
-      <c r="I21" s="5">
-        <v>8.9040649999999992</v>
+      <c r="I21" s="17">
+        <v>0.81</v>
       </c>
       <c r="J21" s="5">
         <v>8.9028435403632997</v>
@@ -1278,7 +1399,7 @@
       <c r="H22" s="5">
         <v>0</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="18">
         <v>1.3312022998777736E-2</v>
       </c>
       <c r="J22" s="5">
@@ -1313,7 +1434,7 @@
       <c r="H23" s="5">
         <v>0</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="16">
         <v>1.5707160000000001E-2</v>
       </c>
       <c r="J23" s="5">
@@ -1348,7 +1469,7 @@
       <c r="H24" s="5">
         <v>0</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="16">
         <v>1.5707160000000001E-2</v>
       </c>
       <c r="J24" s="5">
@@ -1383,7 +1504,7 @@
       <c r="H25" s="5">
         <v>0</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="19">
         <v>1283.9739999999999</v>
       </c>
       <c r="J25" s="5">
@@ -1418,7 +1539,7 @@
       <c r="H26" s="5">
         <v>0</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="18">
         <v>1.7971797</v>
       </c>
       <c r="J26" s="5">
@@ -1453,7 +1574,7 @@
       <c r="H27" s="5">
         <v>5.4416944769585003</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="19">
         <v>3798.9149750000001</v>
       </c>
       <c r="J27" s="5">
@@ -1488,7 +1609,7 @@
       <c r="H28" s="5">
         <v>0</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="16">
         <v>2.8824099999999998E-2</v>
       </c>
       <c r="J28" s="5">
@@ -1523,7 +1644,7 @@
       <c r="H29" s="5">
         <v>0</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="16">
         <v>2.8824099999999998E-2</v>
       </c>
       <c r="J29" s="5">
@@ -1558,7 +1679,7 @@
       <c r="H30" s="5">
         <v>0</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="19">
         <v>2449.3220000000001</v>
       </c>
       <c r="J30" s="5">
@@ -1593,7 +1714,7 @@
       <c r="H31" s="5">
         <v>0</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="17">
         <v>2.1</v>
       </c>
       <c r="J31" s="5">
@@ -1628,8 +1749,8 @@
       <c r="H32" s="5">
         <v>0</v>
       </c>
-      <c r="I32" s="5">
-        <v>9.3475249999999992</v>
+      <c r="I32" s="17">
+        <v>0.82</v>
       </c>
       <c r="J32" s="5">
         <v>9.3701874200357498</v>
@@ -1639,199 +1760,529 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="4"/>
+      <c r="A33" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="10">
+        <v>1.2368489999997E-2</v>
+      </c>
+      <c r="F33" s="11">
+        <v>7.3880179522547058</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0</v>
+      </c>
+      <c r="I33" s="20">
+        <v>1.2368489999997E-2</v>
+      </c>
+      <c r="J33" s="11">
+        <v>7.3880179522547058</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="4"/>
+      <c r="A34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0.1387311</v>
+      </c>
+      <c r="F34" s="11">
+        <v>82.828872031619994</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11">
+        <v>0</v>
+      </c>
+      <c r="I34" s="20">
+        <v>0.1387311</v>
+      </c>
+      <c r="J34" s="11">
+        <v>82.828872031619994</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="4"/>
+      <c r="A35" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="12">
+        <v>285.98899999999998</v>
+      </c>
+      <c r="F35" s="11">
+        <v>82.828872031619994</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1.429945</v>
+      </c>
+      <c r="H35" s="11">
+        <v>0.41414436015810002</v>
+      </c>
+      <c r="I35" s="20">
+        <v>284.559055</v>
+      </c>
+      <c r="J35" s="11">
+        <v>82.414727671461904</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="4"/>
+      <c r="A36" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="10">
+        <v>6.0019999999999998</v>
+      </c>
+      <c r="F36" s="11">
+        <v>3598.9702946325401</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11">
+        <v>0</v>
+      </c>
+      <c r="I36" s="20">
+        <v>6.0019999999999998</v>
+      </c>
+      <c r="J36" s="11">
+        <v>3598.9702946325401</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="4"/>
+      <c r="A37" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="10">
+        <v>6.0019999999999998</v>
+      </c>
+      <c r="F37" s="11">
+        <v>3612.4230731777102</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0</v>
+      </c>
+      <c r="I37" s="20">
+        <v>6.0019999999999998</v>
+      </c>
+      <c r="J37" s="11">
+        <v>3612.4230731777102</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="4"/>
+      <c r="A38" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="12">
+        <v>12406.581</v>
+      </c>
+      <c r="F38" s="11">
+        <v>3612.4230731777102</v>
+      </c>
+      <c r="G38" s="10">
+        <v>62.032905</v>
+      </c>
+      <c r="H38" s="11">
+        <v>18.062115365888548</v>
+      </c>
+      <c r="I38" s="20">
+        <v>12344.548095</v>
+      </c>
+      <c r="J38" s="11">
+        <v>3594.3609578118217</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="4"/>
+      <c r="A39" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="11">
+        <v>9.3925929999999997</v>
+      </c>
+      <c r="F39" s="11">
+        <v>9.4118555175762602</v>
+      </c>
+      <c r="G39" s="11">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0</v>
+      </c>
+      <c r="I39" s="20">
+        <v>0.78</v>
+      </c>
+      <c r="J39" s="11">
+        <v>9.4118555175762602</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="4"/>
+      <c r="A40" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="11">
+        <v>8.5924069999999997</v>
+      </c>
+      <c r="F40" s="11">
+        <v>8.5803597579934401</v>
+      </c>
+      <c r="G40" s="11">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11">
+        <v>0</v>
+      </c>
+      <c r="I40" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="J40" s="11">
+        <v>8.5803597579934401</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="4"/>
+      <c r="A41" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0.246533841787</v>
+      </c>
+      <c r="F41" s="11">
+        <v>158.05914650191198</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11">
+        <v>0</v>
+      </c>
+      <c r="I41" s="20">
+        <v>0.246533841787</v>
+      </c>
+      <c r="J41" s="11">
+        <v>158.05914650191198</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="4"/>
+      <c r="A42" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0.2465338</v>
+      </c>
+      <c r="F42" s="11">
+        <v>157.86375042492</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0</v>
+      </c>
+      <c r="H42" s="11">
+        <v>0</v>
+      </c>
+      <c r="I42" s="20">
+        <v>0.2465338</v>
+      </c>
+      <c r="J42" s="11">
+        <v>157.86375042492</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="4"/>
+      <c r="A43" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="12">
+        <v>494.16300000000001</v>
+      </c>
+      <c r="F43" s="11">
+        <v>157.86375042492</v>
+      </c>
+      <c r="G43" s="10">
+        <v>2.470815</v>
+      </c>
+      <c r="H43" s="11">
+        <v>0.78931875212460001</v>
+      </c>
+      <c r="I43" s="20">
+        <v>491.69218499999999</v>
+      </c>
+      <c r="J43" s="11">
+        <v>157.07443167279541</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="4"/>
+      <c r="A44" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="11">
+        <v>8.2928840000000008</v>
+      </c>
+      <c r="F44" s="11">
+        <v>8.2643126926124797</v>
+      </c>
+      <c r="G44" s="11">
+        <v>0</v>
+      </c>
+      <c r="H44" s="11">
+        <v>0</v>
+      </c>
+      <c r="I44" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="J44" s="11">
+        <v>8.2643126926124797</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="4"/>
+      <c r="A45" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="11">
+        <v>8.3102180000000008</v>
+      </c>
+      <c r="F45" s="11">
+        <v>8.3022777529053595</v>
+      </c>
+      <c r="G45" s="11">
+        <v>0</v>
+      </c>
+      <c r="H45" s="11">
+        <v>0</v>
+      </c>
+      <c r="I45" s="20">
+        <v>2.75</v>
+      </c>
+      <c r="J45" s="11">
+        <v>8.3022777529053595</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="4"/>
+      <c r="A46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="11">
+        <v>8.3137369999999997</v>
+      </c>
+      <c r="F46" s="11">
+        <v>8.32533591017555</v>
+      </c>
+      <c r="G46" s="11">
+        <v>0</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
+      <c r="I46" s="20">
+        <v>4</v>
+      </c>
+      <c r="J46" s="11">
+        <v>8.32533591017555</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="4"/>
+      <c r="A47" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="11">
+        <v>8.4554670000000005</v>
+      </c>
+      <c r="F47" s="11">
+        <v>8.4628827827776796</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0</v>
+      </c>
+      <c r="H47" s="11">
+        <v>0</v>
+      </c>
+      <c r="I47" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J47" s="11">
+        <v>8.4628827827776796</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" s="4"/>
@@ -1842,7 +2293,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="7"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="7"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="5"/>
       <c r="K48" s="4"/>
     </row>
@@ -1855,7 +2306,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="8"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="8"/>
+      <c r="I49" s="16"/>
       <c r="J49" s="5"/>
       <c r="K49" s="4"/>
     </row>
@@ -1868,7 +2319,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="I50" s="17"/>
       <c r="J50" s="5"/>
       <c r="K50" s="4"/>
     </row>
@@ -1881,7 +2332,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="I51" s="17"/>
       <c r="J51" s="5"/>
       <c r="K51" s="4"/>
     </row>
@@ -1894,7 +2345,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
+      <c r="I52" s="17"/>
       <c r="J52" s="5"/>
       <c r="K52" s="4"/>
     </row>
@@ -1907,7 +2358,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
+      <c r="I53" s="17"/>
       <c r="J53" s="5"/>
       <c r="K53" s="4"/>
     </row>
@@ -1920,7 +2371,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
+      <c r="I54" s="17"/>
       <c r="J54" s="5"/>
       <c r="K54" s="4"/>
     </row>
@@ -1933,7 +2384,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
+      <c r="I55" s="17"/>
       <c r="J55" s="5"/>
       <c r="K55" s="4"/>
     </row>
@@ -1946,7 +2397,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
+      <c r="I56" s="17"/>
       <c r="J56" s="5"/>
       <c r="K56" s="4"/>
     </row>
@@ -1959,7 +2410,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+      <c r="I57" s="17"/>
       <c r="J57" s="5"/>
       <c r="K57" s="4"/>
     </row>
@@ -1972,7 +2423,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="I58" s="17"/>
       <c r="J58" s="5"/>
       <c r="K58" s="4"/>
     </row>
@@ -1985,7 +2436,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="I59" s="17"/>
       <c r="J59" s="5"/>
       <c r="K59" s="4"/>
     </row>
@@ -1998,7 +2449,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="I60" s="17"/>
       <c r="J60" s="5"/>
       <c r="K60" s="4"/>
     </row>
@@ -2011,7 +2462,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="I61" s="17"/>
       <c r="J61" s="5"/>
       <c r="K61" s="4"/>
     </row>
@@ -2024,7 +2475,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="I62" s="17"/>
       <c r="J62" s="5"/>
       <c r="K62" s="4"/>
     </row>
@@ -2037,7 +2488,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="I63" s="17"/>
       <c r="J63" s="5"/>
       <c r="K63" s="4"/>
     </row>
@@ -2050,7 +2501,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="I64" s="17"/>
       <c r="J64" s="5"/>
       <c r="K64" s="4"/>
     </row>
@@ -2063,7 +2514,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="I65" s="17"/>
       <c r="J65" s="5"/>
       <c r="K65" s="4"/>
     </row>
@@ -2076,7 +2527,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
+      <c r="I66" s="17"/>
       <c r="J66" s="5"/>
       <c r="K66" s="4"/>
     </row>
@@ -2089,7 +2540,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
+      <c r="I67" s="17"/>
       <c r="J67" s="5"/>
       <c r="K67" s="4"/>
     </row>
@@ -2102,7 +2553,7 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="I68" s="17"/>
       <c r="J68" s="5"/>
       <c r="K68" s="4"/>
     </row>
@@ -2115,7 +2566,7 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
+      <c r="I69" s="17"/>
       <c r="J69" s="5"/>
       <c r="K69" s="4"/>
     </row>
@@ -2128,7 +2579,7 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
+      <c r="I70" s="17"/>
       <c r="J70" s="5"/>
       <c r="K70" s="4"/>
     </row>
@@ -2141,7 +2592,7 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="I71" s="17"/>
       <c r="J71" s="5"/>
       <c r="K71" s="4"/>
     </row>
@@ -2154,7 +2605,7 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="I72" s="17"/>
       <c r="J72" s="5"/>
       <c r="K72" s="4"/>
     </row>
@@ -2167,7 +2618,7 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="I73" s="17"/>
       <c r="J73" s="5"/>
       <c r="K73" s="4"/>
     </row>
@@ -2180,7 +2631,7 @@
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="I74" s="17"/>
       <c r="J74" s="5"/>
       <c r="K74" s="4"/>
     </row>
@@ -2193,7 +2644,7 @@
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="I75" s="17"/>
       <c r="J75" s="5"/>
       <c r="K75" s="4"/>
     </row>
@@ -2206,7 +2657,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="I76" s="17"/>
       <c r="J76" s="5"/>
       <c r="K76" s="4"/>
     </row>
@@ -2219,7 +2670,7 @@
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="I77" s="17"/>
       <c r="J77" s="5"/>
       <c r="K77" s="4"/>
     </row>
@@ -2232,7 +2683,7 @@
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="I78" s="17"/>
       <c r="J78" s="5"/>
       <c r="K78" s="4"/>
     </row>
@@ -2245,7 +2696,7 @@
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="I79" s="17"/>
       <c r="J79" s="5"/>
       <c r="K79" s="4"/>
     </row>
@@ -2258,7 +2709,7 @@
       <c r="F80" s="5"/>
       <c r="G80" s="7"/>
       <c r="H80" s="5"/>
-      <c r="I80" s="7"/>
+      <c r="I80" s="19"/>
       <c r="J80" s="5"/>
       <c r="K80" s="4"/>
     </row>
@@ -2271,7 +2722,7 @@
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="I81" s="17"/>
       <c r="J81" s="5"/>
       <c r="K81" s="4"/>
     </row>
@@ -2284,7 +2735,7 @@
       <c r="F82" s="5"/>
       <c r="G82" s="7"/>
       <c r="H82" s="5"/>
-      <c r="I82" s="7"/>
+      <c r="I82" s="19"/>
       <c r="J82" s="5"/>
       <c r="K82" s="4"/>
     </row>
@@ -2297,7 +2748,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
+      <c r="I83" s="17"/>
       <c r="J83" s="5"/>
       <c r="K83" s="4"/>
     </row>
@@ -2310,7 +2761,7 @@
       <c r="F84" s="5"/>
       <c r="G84" s="7"/>
       <c r="H84" s="5"/>
-      <c r="I84" s="7"/>
+      <c r="I84" s="19"/>
       <c r="J84" s="5"/>
       <c r="K84" s="4"/>
     </row>
@@ -2323,7 +2774,7 @@
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="I85" s="17"/>
       <c r="J85" s="5"/>
       <c r="K85" s="4"/>
     </row>
@@ -2336,7 +2787,7 @@
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
+      <c r="I86" s="17"/>
       <c r="J86" s="5"/>
       <c r="K86" s="4"/>
     </row>
@@ -2349,7 +2800,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="7"/>
       <c r="H87" s="5"/>
-      <c r="I87" s="7"/>
+      <c r="I87" s="19"/>
       <c r="J87" s="5"/>
       <c r="K87" s="4"/>
     </row>
@@ -2362,7 +2813,7 @@
       <c r="F88" s="5"/>
       <c r="G88" s="7"/>
       <c r="H88" s="5"/>
-      <c r="I88" s="7"/>
+      <c r="I88" s="19"/>
       <c r="J88" s="5"/>
       <c r="K88" s="4"/>
     </row>
@@ -2375,7 +2826,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
+      <c r="I89" s="17"/>
       <c r="J89" s="5"/>
       <c r="K89" s="4"/>
     </row>
@@ -2388,7 +2839,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
+      <c r="I90" s="17"/>
       <c r="J90" s="5"/>
       <c r="K90" s="4"/>
     </row>
@@ -2401,7 +2852,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
+      <c r="I91" s="17"/>
       <c r="J91" s="5"/>
       <c r="K91" s="4"/>
     </row>
@@ -2414,7 +2865,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
-      <c r="I92" s="6"/>
+      <c r="I92" s="18"/>
       <c r="J92" s="5"/>
       <c r="K92" s="4"/>
     </row>
@@ -2427,7 +2878,7 @@
       <c r="F93" s="5"/>
       <c r="G93" s="7"/>
       <c r="H93" s="5"/>
-      <c r="I93" s="7"/>
+      <c r="I93" s="19"/>
       <c r="J93" s="5"/>
       <c r="K93" s="4"/>
     </row>
@@ -2440,7 +2891,7 @@
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
+      <c r="I94" s="17"/>
       <c r="J94" s="5"/>
       <c r="K94" s="4"/>
     </row>
@@ -2453,7 +2904,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="7"/>
       <c r="H95" s="5"/>
-      <c r="I95" s="7"/>
+      <c r="I95" s="19"/>
       <c r="J95" s="5"/>
       <c r="K95" s="4"/>
     </row>
@@ -2466,7 +2917,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
+      <c r="I96" s="17"/>
       <c r="J96" s="5"/>
       <c r="K96" s="4"/>
     </row>
@@ -2479,7 +2930,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="7"/>
       <c r="H97" s="5"/>
-      <c r="I97" s="7"/>
+      <c r="I97" s="19"/>
       <c r="J97" s="5"/>
       <c r="K97" s="4"/>
     </row>
@@ -2492,7 +2943,7 @@
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
+      <c r="I98" s="17"/>
       <c r="J98" s="5"/>
       <c r="K98" s="4"/>
     </row>
@@ -2505,7 +2956,7 @@
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
+      <c r="I99" s="17"/>
       <c r="J99" s="5"/>
       <c r="K99" s="4"/>
     </row>
@@ -2518,7 +2969,7 @@
       <c r="F100" s="5"/>
       <c r="G100" s="7"/>
       <c r="H100" s="5"/>
-      <c r="I100" s="7"/>
+      <c r="I100" s="19"/>
       <c r="J100" s="5"/>
       <c r="K100" s="4"/>
     </row>
@@ -2531,7 +2982,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
+      <c r="I101" s="17"/>
       <c r="J101" s="5"/>
       <c r="K101" s="4"/>
     </row>
@@ -2544,7 +2995,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="7"/>
       <c r="H102" s="5"/>
-      <c r="I102" s="7"/>
+      <c r="I102" s="19"/>
       <c r="J102" s="5"/>
       <c r="K102" s="4"/>
     </row>
@@ -2557,7 +3008,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
+      <c r="I103" s="17"/>
       <c r="J103" s="5"/>
       <c r="K103" s="4"/>
     </row>
@@ -2570,7 +3021,7 @@
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
+      <c r="I104" s="17"/>
       <c r="J104" s="5"/>
       <c r="K104" s="4"/>
     </row>
@@ -2583,7 +3034,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
-      <c r="I105" s="6"/>
+      <c r="I105" s="18"/>
       <c r="J105" s="5"/>
       <c r="K105" s="4"/>
     </row>
@@ -2596,7 +3047,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
+      <c r="I106" s="17"/>
       <c r="J106" s="5"/>
       <c r="K106" s="4"/>
     </row>
@@ -2609,7 +3060,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="7"/>
       <c r="H107" s="5"/>
-      <c r="I107" s="7"/>
+      <c r="I107" s="19"/>
       <c r="J107" s="5"/>
       <c r="K107" s="4"/>
     </row>
@@ -2622,7 +3073,7 @@
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
       <c r="H108" s="5"/>
-      <c r="I108" s="5"/>
+      <c r="I108" s="17"/>
       <c r="J108" s="5"/>
       <c r="K108" s="4"/>
     </row>
@@ -2635,7 +3086,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="7"/>
       <c r="H109" s="5"/>
-      <c r="I109" s="7"/>
+      <c r="I109" s="19"/>
       <c r="J109" s="5"/>
       <c r="K109" s="4"/>
     </row>
@@ -2648,7 +3099,7 @@
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
-      <c r="I110" s="5"/>
+      <c r="I110" s="17"/>
       <c r="J110" s="5"/>
       <c r="K110" s="4"/>
     </row>
@@ -2661,7 +3112,7 @@
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
       <c r="H111" s="5"/>
-      <c r="I111" s="8"/>
+      <c r="I111" s="16"/>
       <c r="J111" s="5"/>
       <c r="K111" s="4"/>
     </row>
@@ -2674,7 +3125,7 @@
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
-      <c r="I112" s="5"/>
+      <c r="I112" s="17"/>
       <c r="J112" s="5"/>
       <c r="K112" s="4"/>
     </row>
@@ -2687,7 +3138,7 @@
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
-      <c r="I113" s="6"/>
+      <c r="I113" s="18"/>
       <c r="J113" s="5"/>
       <c r="K113" s="4"/>
     </row>
@@ -2700,7 +3151,7 @@
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
       <c r="H114" s="5"/>
-      <c r="I114" s="5"/>
+      <c r="I114" s="17"/>
       <c r="J114" s="5"/>
       <c r="K114" s="4"/>
     </row>
@@ -2713,7 +3164,7 @@
       <c r="F115" s="5"/>
       <c r="G115" s="7"/>
       <c r="H115" s="5"/>
-      <c r="I115" s="7"/>
+      <c r="I115" s="19"/>
       <c r="J115" s="5"/>
       <c r="K115" s="4"/>
     </row>
@@ -2726,7 +3177,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="7"/>
       <c r="H116" s="5"/>
-      <c r="I116" s="7"/>
+      <c r="I116" s="19"/>
       <c r="J116" s="5"/>
       <c r="K116" s="4"/>
     </row>
@@ -2739,7 +3190,7 @@
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
       <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
+      <c r="I117" s="17"/>
       <c r="J117" s="5"/>
       <c r="K117" s="4"/>
     </row>
@@ -2752,7 +3203,7 @@
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="5"/>
-      <c r="I118" s="5"/>
+      <c r="I118" s="17"/>
       <c r="J118" s="5"/>
       <c r="K118" s="4"/>
     </row>
@@ -2765,7 +3216,7 @@
       <c r="F119" s="5"/>
       <c r="G119" s="7"/>
       <c r="H119" s="5"/>
-      <c r="I119" s="7"/>
+      <c r="I119" s="19"/>
       <c r="J119" s="5"/>
       <c r="K119" s="4"/>
     </row>
@@ -2778,7 +3229,7 @@
       <c r="F120" s="5"/>
       <c r="G120" s="7"/>
       <c r="H120" s="5"/>
-      <c r="I120" s="7"/>
+      <c r="I120" s="19"/>
       <c r="J120" s="5"/>
       <c r="K120" s="4"/>
     </row>
@@ -2791,7 +3242,7 @@
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
-      <c r="I121" s="5"/>
+      <c r="I121" s="17"/>
       <c r="J121" s="5"/>
       <c r="K121" s="4"/>
     </row>
@@ -2804,7 +3255,7 @@
       <c r="F122" s="5"/>
       <c r="G122" s="7"/>
       <c r="H122" s="5"/>
-      <c r="I122" s="7"/>
+      <c r="I122" s="19"/>
       <c r="J122" s="5"/>
       <c r="K122" s="4"/>
     </row>
@@ -2817,7 +3268,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
-      <c r="I123" s="5"/>
+      <c r="I123" s="17"/>
       <c r="J123" s="5"/>
       <c r="K123" s="4"/>
     </row>
@@ -2830,7 +3281,7 @@
       <c r="F124" s="5"/>
       <c r="G124" s="7"/>
       <c r="H124" s="5"/>
-      <c r="I124" s="7"/>
+      <c r="I124" s="19"/>
       <c r="J124" s="5"/>
       <c r="K124" s="4"/>
     </row>
@@ -2843,7 +3294,7 @@
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
-      <c r="I125" s="5"/>
+      <c r="I125" s="17"/>
       <c r="J125" s="5"/>
       <c r="K125" s="4"/>
     </row>
@@ -2856,7 +3307,7 @@
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
-      <c r="I126" s="5"/>
+      <c r="I126" s="17"/>
       <c r="J126" s="5"/>
       <c r="K126" s="4"/>
     </row>
@@ -2869,7 +3320,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="7"/>
       <c r="H127" s="5"/>
-      <c r="I127" s="7"/>
+      <c r="I127" s="19"/>
       <c r="J127" s="5"/>
       <c r="K127" s="4"/>
     </row>
@@ -2882,7 +3333,7 @@
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
       <c r="H128" s="5"/>
-      <c r="I128" s="5"/>
+      <c r="I128" s="17"/>
       <c r="J128" s="5"/>
       <c r="K128" s="4"/>
     </row>
@@ -2895,7 +3346,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
-      <c r="I129" s="5"/>
+      <c r="I129" s="17"/>
       <c r="J129" s="5"/>
       <c r="K129" s="4"/>
     </row>
@@ -2908,7 +3359,7 @@
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
       <c r="H130" s="5"/>
-      <c r="I130" s="7"/>
+      <c r="I130" s="19"/>
       <c r="J130" s="5"/>
       <c r="K130" s="4"/>
     </row>
@@ -2921,7 +3372,7 @@
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
-      <c r="I131" s="5"/>
+      <c r="I131" s="17"/>
       <c r="J131" s="5"/>
       <c r="K131" s="4"/>
     </row>
@@ -2934,7 +3385,7 @@
       <c r="F132" s="5"/>
       <c r="G132" s="7"/>
       <c r="H132" s="5"/>
-      <c r="I132" s="7"/>
+      <c r="I132" s="19"/>
       <c r="J132" s="5"/>
       <c r="K132" s="4"/>
     </row>
@@ -2947,7 +3398,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
-      <c r="I133" s="5"/>
+      <c r="I133" s="17"/>
       <c r="J133" s="5"/>
       <c r="K133" s="4"/>
     </row>
@@ -2960,7 +3411,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
       <c r="H134" s="5"/>
-      <c r="I134" s="5"/>
+      <c r="I134" s="17"/>
       <c r="J134" s="5"/>
       <c r="K134" s="4"/>
     </row>
@@ -2973,7 +3424,7 @@
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
       <c r="H135" s="5"/>
-      <c r="I135" s="5"/>
+      <c r="I135" s="17"/>
       <c r="J135" s="5"/>
       <c r="K135" s="4"/>
     </row>
@@ -2986,7 +3437,7 @@
       <c r="F136" s="5"/>
       <c r="G136" s="7"/>
       <c r="H136" s="5"/>
-      <c r="I136" s="7"/>
+      <c r="I136" s="19"/>
       <c r="J136" s="5"/>
       <c r="K136" s="4"/>
     </row>
@@ -2999,7 +3450,7 @@
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
-      <c r="I137" s="5"/>
+      <c r="I137" s="17"/>
       <c r="J137" s="5"/>
       <c r="K137" s="4"/>
     </row>
@@ -3012,7 +3463,7 @@
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
       <c r="H138" s="5"/>
-      <c r="I138" s="5"/>
+      <c r="I138" s="17"/>
       <c r="J138" s="5"/>
       <c r="K138" s="4"/>
     </row>
@@ -3025,7 +3476,7 @@
       <c r="F139" s="5"/>
       <c r="G139" s="7"/>
       <c r="H139" s="5"/>
-      <c r="I139" s="7"/>
+      <c r="I139" s="19"/>
       <c r="J139" s="5"/>
       <c r="K139" s="4"/>
     </row>
@@ -3038,7 +3489,7 @@
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
       <c r="H140" s="5"/>
-      <c r="I140" s="5"/>
+      <c r="I140" s="17"/>
       <c r="J140" s="5"/>
       <c r="K140" s="4"/>
     </row>
@@ -3051,7 +3502,7 @@
       <c r="F141" s="5"/>
       <c r="G141" s="7"/>
       <c r="H141" s="5"/>
-      <c r="I141" s="7"/>
+      <c r="I141" s="19"/>
       <c r="J141" s="5"/>
       <c r="K141" s="4"/>
     </row>
@@ -3064,7 +3515,7 @@
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
       <c r="H142" s="5"/>
-      <c r="I142" s="5"/>
+      <c r="I142" s="17"/>
       <c r="J142" s="5"/>
       <c r="K142" s="4"/>
     </row>
@@ -3077,7 +3528,7 @@
       <c r="F143" s="5"/>
       <c r="G143" s="7"/>
       <c r="H143" s="5"/>
-      <c r="I143" s="7"/>
+      <c r="I143" s="19"/>
       <c r="J143" s="5"/>
       <c r="K143" s="4"/>
     </row>
@@ -3090,7 +3541,7 @@
       <c r="F144" s="5"/>
       <c r="G144" s="7"/>
       <c r="H144" s="5"/>
-      <c r="I144" s="7"/>
+      <c r="I144" s="19"/>
       <c r="J144" s="5"/>
       <c r="K144" s="4"/>
     </row>
@@ -3103,7 +3554,7 @@
       <c r="F145" s="5"/>
       <c r="G145" s="5"/>
       <c r="H145" s="5"/>
-      <c r="I145" s="5"/>
+      <c r="I145" s="17"/>
       <c r="J145" s="5"/>
       <c r="K145" s="4"/>
     </row>
@@ -3116,7 +3567,7 @@
       <c r="F146" s="5"/>
       <c r="G146" s="7"/>
       <c r="H146" s="5"/>
-      <c r="I146" s="7"/>
+      <c r="I146" s="19"/>
       <c r="J146" s="5"/>
       <c r="K146" s="4"/>
     </row>
@@ -3129,7 +3580,7 @@
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
       <c r="H147" s="5"/>
-      <c r="I147" s="5"/>
+      <c r="I147" s="17"/>
       <c r="J147" s="5"/>
       <c r="K147" s="4"/>
     </row>
@@ -3142,7 +3593,7 @@
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
       <c r="H148" s="5"/>
-      <c r="I148" s="5"/>
+      <c r="I148" s="17"/>
       <c r="J148" s="5"/>
       <c r="K148" s="4"/>
     </row>
@@ -3155,7 +3606,7 @@
       <c r="F149" s="5"/>
       <c r="G149" s="7"/>
       <c r="H149" s="5"/>
-      <c r="I149" s="7"/>
+      <c r="I149" s="19"/>
       <c r="J149" s="5"/>
       <c r="K149" s="4"/>
     </row>
@@ -3168,7 +3619,7 @@
       <c r="F150" s="5"/>
       <c r="G150" s="5"/>
       <c r="H150" s="5"/>
-      <c r="I150" s="5"/>
+      <c r="I150" s="17"/>
       <c r="J150" s="5"/>
       <c r="K150" s="4"/>
     </row>
@@ -3181,7 +3632,7 @@
       <c r="F151" s="5"/>
       <c r="G151" s="7"/>
       <c r="H151" s="5"/>
-      <c r="I151" s="7"/>
+      <c r="I151" s="19"/>
       <c r="J151" s="5"/>
       <c r="K151" s="4"/>
     </row>
@@ -3194,7 +3645,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
       <c r="H152" s="5"/>
-      <c r="I152" s="5"/>
+      <c r="I152" s="17"/>
       <c r="J152" s="5"/>
       <c r="K152" s="4"/>
     </row>
@@ -3207,7 +3658,7 @@
       <c r="F153" s="5"/>
       <c r="G153" s="7"/>
       <c r="H153" s="5"/>
-      <c r="I153" s="7"/>
+      <c r="I153" s="19"/>
       <c r="J153" s="5"/>
       <c r="K153" s="4"/>
     </row>
@@ -3220,7 +3671,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="7"/>
       <c r="H154" s="5"/>
-      <c r="I154" s="7"/>
+      <c r="I154" s="19"/>
       <c r="J154" s="5"/>
       <c r="K154" s="4"/>
     </row>
@@ -3233,7 +3684,7 @@
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
       <c r="H155" s="5"/>
-      <c r="I155" s="5"/>
+      <c r="I155" s="17"/>
       <c r="J155" s="5"/>
       <c r="K155" s="4"/>
     </row>
@@ -3243,6 +3694,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>